<commit_message>
Updated BOM with some fresh JLC codes
</commit_message>
<xml_diff>
--- a/DSpeed_v1.3/DStage_ETC_v1.3_BOM.xlsx
+++ b/DSpeed_v1.3/DStage_ETC_v1.3_BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="178">
   <si>
     <t>Comment</t>
   </si>
@@ -532,7 +532,10 @@
     <t>SMD-3_3.0x3.8x1.2</t>
   </si>
   <si>
-    <t>C128545</t>
+    <t>C719186</t>
+  </si>
+  <si>
+    <t>updated from C128545</t>
   </si>
   <si>
     <t>270R</t>
@@ -612,7 +615,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -687,6 +690,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -1805,77 +1811,79 @@
       <c r="C51" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="D51" s="6" t="s">
+      <c r="D51" s="27" t="s">
         <v>172</v>
       </c>
-      <c r="E51" s="10"/>
+      <c r="E51" s="7" t="s">
+        <v>173</v>
+      </c>
       <c r="F51" s="8"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="11" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C52" s="12" t="s">
         <v>36</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F52" s="8"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="27"/>
-      <c r="B53" s="27"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="29"/>
+      <c r="A53" s="28"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="30"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="30"/>
-      <c r="B54" s="30"/>
-      <c r="C54" s="31"/>
-      <c r="D54" s="32"/>
+      <c r="A54" s="31"/>
+      <c r="B54" s="31"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="33"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="27"/>
-      <c r="B55" s="27"/>
-      <c r="C55" s="28"/>
-      <c r="D55" s="29"/>
+      <c r="A55" s="28"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="29"/>
+      <c r="D55" s="30"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="30"/>
-      <c r="B56" s="30"/>
-      <c r="C56" s="31"/>
-      <c r="D56" s="32"/>
+      <c r="A56" s="31"/>
+      <c r="B56" s="31"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="33"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="27"/>
-      <c r="B57" s="27"/>
-      <c r="C57" s="28"/>
-      <c r="D57" s="29"/>
+      <c r="A57" s="28"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="29"/>
+      <c r="D57" s="30"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="30"/>
-      <c r="B58" s="30"/>
-      <c r="C58" s="31"/>
-      <c r="D58" s="32"/>
+      <c r="A58" s="31"/>
+      <c r="B58" s="31"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="33"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="27"/>
-      <c r="B59" s="27"/>
-      <c r="C59" s="28"/>
-      <c r="D59" s="29"/>
+      <c r="A59" s="28"/>
+      <c r="B59" s="28"/>
+      <c r="C59" s="29"/>
+      <c r="D59" s="30"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="30"/>
-      <c r="B60" s="30"/>
-      <c r="C60" s="31"/>
-      <c r="D60" s="32"/>
+      <c r="A60" s="31"/>
+      <c r="B60" s="31"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="33"/>
     </row>
     <row r="61" ht="15.75" customHeight="1"/>
     <row r="62" ht="15.75" customHeight="1"/>

</xml_diff>